<commit_message>
se mapeo con el xml para que la informacion sea mas dinamica
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbarajas\Documents\Curses\Bots\BotEmail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FDFEC43-AB62-427E-B824-9191C69A46E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8454D8B-96C8-4AD4-8A24-E7EAE9E708E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="29025" windowHeight="11385" xr2:uid="{F9E33BDC-5FCC-4B3D-8246-DFD7CF1F8D5D}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="29025" windowHeight="11385" xr2:uid="{0D92A2B1-DF0A-4FB0-892B-7298E7EA029F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -508,7 +508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C55270-7971-4229-99F6-A0CE94CC04CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490AF53B-F01D-42D6-8B35-A406A79463A0}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Se cargaron todos los elemntos finales
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbarajas\Documents\Curses\Bots\BotEmail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8454D8B-96C8-4AD4-8A24-E7EAE9E708E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABDBE07-6519-48B2-B5D9-3754C1969BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="29025" windowHeight="11385" xr2:uid="{0D92A2B1-DF0A-4FB0-892B-7298E7EA029F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38940" windowHeight="15840" xr2:uid="{0D92A2B1-DF0A-4FB0-892B-7298E7EA029F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Subject</t>
   </si>
@@ -64,96 +64,6 @@
   </si>
   <si>
     <t>SendDate</t>
-  </si>
-  <si>
-    <t>Weekly Learning Digest</t>
-  </si>
-  <si>
-    <t>CapgeminiNEXT-noreply@degreed.com</t>
-  </si>
-  <si>
-    <t>BARAJAS ARIAS, GUILLERMO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This mail has been sent from an external source	_x000D_
- &lt;https://prod.degreedcdn.com/content/img/org/421-2c6e3e82-a1cb-4592-bda5-40303fd22fab.png&gt; 	_x000D_
-Hi GUILLERMO, here's your weekly digest	 _x000D_
- &lt;https://prod.degreedcdn.com/content/img/email/babycenter/divider-gray.png&gt; _x000D_
-	_x000D_
-What to Learn Next: _x000D_
-Here's what people at Capgemini NEXT are learning this week 	View All &lt;https://email.notifications.degreed.com/c/eJx9UUFuwyAQfI19qWIBJiQcOESqcq5UqT1aa1g7NAYswI3c15dEaZVeKnFYZjS7s7PoP20M3qHP6iUGs-hsg69RUSGkpFRKXqMDO3V5nVG9I56n9el1cQ7iWrWHpweRVYwwRhmhVBC53TfA5Fa2wI3hsiecV5z4kO1gNVwFqTE4RkTT6ODqkyIDbwWjAmAPw0AG3XNKBJVCE9PvhrZeEsZujmGwE3ZnXBXlO0LFTtaTOuU8p2KoYsfyHhqXn8MrBOnUB4imao8hjimFqn3WMI_orLcVE0t2nUNjF1eI2853UIObwY6-wNcFN5RtCL1zKSxRY2Eut2R-FMHnkmiB3yxeDtN0LGYq1hYbQ6nqMh-8_bql0FmjOKN1VONipwmjC00PET4glbx-Dd4y-nOj_P81jNr3LYhvGvyhLQ&gt;  	_x000D_
-3 Trends Transforming eLearning Course Design &lt;https://email.notifications.degreed.com/c/eJx9UcFqxCAQ_ZrkUrKoMcl68FAoe-qh0EKPYaKTrG3UoKYl_fq6YVu2l4LgzBvezOM9dB8meGfRJfkUvF5VMt6VKGnbCkGpELxEC2bu07agfEV8n7e759VaCFtR39_dkIxkhDHKCKUtEc3xAEw0ogauNRcD4bzgxPlkRqPgQogHjVNA1AflbXmWYuyGhg5j19SEYAcNFa0mR0W5QNoKKNeIoV-CH82M_TtukvKO0LYT5SzPKS0xCyrYKb-bxbmDkIyaMeayrlJAp2P-wMXRB2vcVOGMENylUn4NESuN0UyuqE-6qB_YkYuONaJgrQ9TjD5jCpYJM9dkcE22t6jNavNgN-sKKrAL7HseLs5UlFWEXmcxH1KYJ5-7pT8M71KOIsMvXsMWH6-6ynwYnPnafeuNlpzRMshpNfOMwfrDAAHeIGaHf5Xtrv5JNf2fn5bHoYb2GzY0sww&gt;  _x000D_
- &lt;http://res.cloudinary.com/degreed/image/fetch/c_lfill,d_broken-image_iufgnh.png,h_150,w_150/https://gcp-cdn.anderspink.com/article-images/430e5832f89484723fc8bab08afb3270190a990df934a5cf5e00a13e09c5d6dc.jpg&gt; elearningindustry.com | 12 Dec 2021 | Modern digital education is moving toward a more collaborative and inclusive approach. A perfect example is how companies are offering engaging multilingual eLear… _x000D_
-_x000D_
-Article • 4 Minutes _x000D_
-Business perspective - R&amp;D's potential &lt;https://email.notifications.degreed.com/c/eJx9kUFr7SAQhX9Nsim5RGNMXLh48OjqLR600GWYxEnutFGDmlvSX1_vpS3tpuBCz-E4h2_QXSh4Z9El_T94s0-JvCtRMymVYkwpUaIFWod0bKifEF_W4-5htxbCUTR_7r6FSPOac8ZrxmSt2v4EXLWqAWGMUGMtRCFq5xPNNME1EE8Gl4BoTpO35VkzPvJ56sU81y0DOXHsepzHtpddC13flXvEMGzBz7Ti8IKHZqKrmexUuepzSlvMhQp-n8-3j_PrQgZ9zJdxj-QwxmrDEDfMtS9YhcpUWfEpMyBYi-beFM3fhkvWKK4KLn1YYvRZm2Bb0JKjLO7JDhYN7TYbN0If4gR2A1pclq84Ksarmn140e9hwuy83jh-Jry7zs7yozdwxH8IwZFbyjwYHL3dYA1ktOCsDHrZaV0xWH8aIcAzxIz1q9kN5Y9Vpt-XZnQ_NiDfAb4ury0&gt;  _x000D_
- &lt;http://res.cloudinary.com/degreed/image/fetch/c_lfill,d_broken-image_iufgnh.png,h_150,w_150/https://prod.degreedcdn.com/content/img/org/421/8fdd4f49-016c-4a50-a1f3-9c3f746283b0.jpg%3Fv%3D0010127815&gt; Business perspectives unleashing R&amp;D's potential with William Roze CEO of Capgemini Engineering.… _x000D_
-_x000D_
-Video • 58 Minutes _x000D_
-Learning from Success and Failure &lt;https://email.notifications.degreed.com/c/eJx9kctuwyAQRb_G3lSOAD9ZsKgUZdVFpVbq0hrDxKExYPFo5X59SZRW6aYSC7ijy505g_ZDe2cN2iievVNJRu1siYJ2HeeUct6UaEAvY9xWFG-I52V7eEnGgN-K-vHhzqQFI4xRRijtCG-HHTDe8hoapRo-kaYpGmJd1Ect4WIIO4WzR1Q76Ux5EoOSnNAOZD1NQ69UyzkZOjK0MKi-JnWZAvpx9e6oFxzPuAna9NnQ83IRpxjXkBsq2CGfu4_zC3zUcsGQrwuCt9rO1dE7U4UkJYZQgVXVMQ-ZPBb1QRX1nrK2b3NmwTrn5xBc1iSsMxptdRZTNKNBpZPJhSugmyjBrKBnm-ULjYqyitBbLbjkZU7Yf14x_jicjRl_ll-dgi083VosczBY_XVlNWolGkZLL-aklwW9cbsJPLxDyFR_O7uS_LPJ-P_OlBimGrpvW-auSQ&gt;  _x000D_
- &lt;http://res.cloudinary.com/degreed/image/fetch/c_lfill,d_broken-image_iufgnh.png,h_150,w_150/https://hbr.org/resources/images/products/CL-generic-image-hbrarticle.png&gt; One of the mottoes that Diego Rodriguez and I use at the Stanford d.school is "failure sucks, but instructs." We encourage students to learn from the constant stream of small setbacks and successes th… _x000D_
-_x000D_
-Article • 4 Minutes _x000D_
-Did You Know? _x000D_
-Powered by 	 &lt;https://email.notifications.degreed.com/c/eJx9kLtuwzAMRb_GWgIYetrRoKFL5wIdOhq0RDlq9DBkuYD79XUzpUsBLhzOvYfE_BVqyQlzM2-1uN22UDJBw4ZBa8a0lgQThDi1Y0XzgXiPx-V9Twnq0YmXyxMUDKecM04ZG6hW1x64VlqAdE7qmUrZSZpLCz5Y-AW23uFSEV1vSyI3ozifnfJWS6sYiFG7ET0Iz7gS3DNN9g3rtNbiQ8TpjodhcqRsGDWJ5tbaup1CHX895yn43EipC-Tw_WidgjOSM1LNsocYsabSz1DhE7bTz8K6YAo5PJz-_KT9f70z11nA8AMpi3BP&gt; 	_x000D_
-© 2020-2022 Degreed, All rights reserved_x000D_
-4305 Hacienda Drive, Suite 300, Pleasanton, CA 94588 	_x000D_
-Unsubscribe &lt;https://email.notifications.degreed.com/c/eJx9kE9rhDAQxT-NXspKJsY_OeRQKHsu9NCjTMyo6ZpEEi3YT19daNleCgPDPPg93hvynzYG78iv6jUGs_WrDT4nBXUtJYCUIieHdu7WfSH1TnSb96e3zTmMe1Y-Pz1AVnHGOXAGUDNZtQVyWckShTFCaiZEJpgPqx1sjyeQCkNjJDJFH1w-KcASRNuKlkNjNDJtBsG5Bt2cgoF8SxS7JYbBztTdaFcgGgZ1I_NZTeu6pCNQxq_HPBgf18mdy6dNpz5aTVl5nTBNWfnyY3Epm8sRlPXCIHCqSEiBDZDuOYjKtANUbcbrEMeUwsH1uIzkrLf5IaG3X_dKnTVKcMijGjc7zxRdKDRG_MB0lP9l7oX_PHz9_7VGtbrE-hvU94yo&gt;  | Update settings &lt;https://email.notifications.degreed.com/c/eJx9UMFqxCAU_Jp4WQhqjBsPHgplz4UeegxGX7KvGzWoKaRfX7vQsr0UHg8GZoaZgfCBKQYPoeiXFN1uC8ZAQDMplWJMKUHAG1zHcmyg3wBu63F63b036Wi6p9ODCDWnnDNOGZNU9UNruOpVZ4RzQk1UiEbQEAvOaM23ILcOlgTgWhs9uepBcW7BsmmalXPcCEFhpk6y6jH1AsieIY1bijOuMN7g0EycKZNnRVZ9LWXLNVDDL_UejCvyUF-GUjAslXOJack5Nt2zNdsCHgM2vKuUyvZ7-ElHKs0E_LyjEZ0WnJGklx3XFZKP7WSSeTe5tvr1uTf5s2T5fzOnh6kz8gtc_IRJ&gt;  	_x000D_
- &lt;https://email.notifications.degreed.com/o/eJx9jztOxDAUAE-zblaK3nNsJy5ccAMkCsrIsd-Gx_oTOQlSOD2wFTQcYDQztS2-8KffuZaJo1MSBTk0xlpEa5Wg7DlN-7mSeyW6p_P6cuTs23npn67PrcYj_LCCnQQpUQKiAavHzkurbe9VjMrOoNRFQak73zg8ZFsXaWlEsQs1izensddhQAtAknS0YZiHCBClBozajOLYqE1rqzdONN3pdKgGQDNYQeWDWy2Zyu5-FTW3HJwStVy72Tf_7rfvhuDXhTIXfnj_APv_h9GNc-_NF5EQZgY&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This mail has been sent from an external source	_x000D_
- &lt;https://prod.degreedcdn.com/content/img/org/421-2c6e3e82-a1cb-4592-bda5-40303fd22fab.png&gt; 	_x000D_
-Hi GUILLERMO, here's your weekly digest	 _x000D_
- &lt;https://prod.degreedcdn.com/content/img/email/babycenter/divider-gray.png&gt; _x000D_
-	_x000D_
-What to Learn Next: _x000D_
-Here's what people at Capgemini NEXT are learning this week 	View All &lt;https://email.notifications.degreed.com/c/eJx9UctqwzAQ_Br7UmL0cOT4oEOg5FwotEezkteOGksyktzgfn0Vk5b0UtBhNcPszs6i-zTBO4suyZfg-0Un412JkgrRtpSShpVowUxdWmeU74iXaX16XayFsBb8-PQgMpIRxigjWUbquq1q1DBovtegGkU4FjVxPpnBaLgJYtXjGBD7SntbniWHuhHQ9gLpQQsmkKs9gUGoFkhLW1UuEUM3Bz-YCbsLrpLWDaGiactJnlOaYzZUsFN-D43zz-INgnhWHkJf8JMPY4y-4M8a5hGtcaZgYkm2s9ibxWZi2_kOarAzmNFl-LbgjrIdoXcu-iVozMx1S-ZH4V3KiWb4zeD1OE2nbKZgPNsYclXm-eDM15ZCZ3pZM1oGOS5mmjBYXykI8AEx5_VrcMvoz43S_9fo5UFxEN8jS6Hc&gt;  	_x000D_
-3 Trends Transforming eLearning Course Design &lt;https://email.notifications.degreed.com/c/eJx9UU1r3TAQ_DX2Jfihr_jjoEMg5JRDIIUezVpaO0osyUhyi_vru8-8luQSEGh3ltkdZjD8cikGj6HolxTtboqLoUbN23YYOGedqNGDW8dybKh_In6sx93r7j2ko5IPd59ITgsmBBeMaEyp4aLQwGzkvYGpm5jESrEQi5udgSshXywuCdFeTPT1m5460Vs5CDaI2fR2pgYVByZn4Ez1U71nTOOW4uxWHD_w0Fx1jLfdUK_6rZQtk6BKPNH7tJg6SMWZFTOVsikJg830QchzTN6FpcEVIYVrZeKeMjYWs1tCJZ9sJR9Fr4ZO3A-VaGNaco6EGdgWJK4jcC9-9Gjd7mlwmnUDDfgNzj2PV2caLhrGb7NMhwzS5Pdp6T9GDIWiIPhHtHDk55uumg5DcH9O30ZntRK8TnrZ3bpi8vEyQYJ3yOTwf2Wnq19SLd_nZ3U_SWj_AgJctCw&gt;  _x000D_
- &lt;http://res.cloudinary.com/degreed/image/fetch/c_lfill,d_broken-image_iufgnh.png,h_150,w_150/https://gcp-cdn.anderspink.com/article-images/430e5832f89484723fc8bab08afb3270190a990df934a5cf5e00a13e09c5d6dc.jpg&gt; elearningindustry.com | 12 Dec 2021 | Modern digital education is moving toward a more collaborative and inclusive approach. A perfect example is how companies are offering engaging multilingual eLear… _x000D_
-_x000D_
-Article • 4 Minutes _x000D_
-Business perspective - R&amp;D's potential &lt;https://email.notifications.degreed.com/c/eJx9kc1qwzAQhJ_GvhQH_dhOfNChUHLqodBCj2YtbZxtLMlIcor79FVCWtJLQQdphtEO36I7U_DOokvqJXiz6ETelah423Yd52wrSrRAU5_WGdU74mlaH14XayGshXx8uAuREkwILliOsbruNjVqOGjZaBi2A5NY1Mz5RAfScAnEjcExIJqN9rY8Ki6xEabhemgF27UDhx0OrGNNozsEycolYujn4A80YX_CVfF6y3i77cpJHVOaYy5UiH0-dx_n15kM-pgvwxLJYYzVjCHOmGufsQqVqbLiU2ZAMBVybwr5JEXLZSe6QrQ-jDH6rGmYR7TkKItLsr1FQ4vNxpXQTdRgZ6DRZfmCo-KiYvzmRb8Ejdn5vHL8SXh3mZ3lN29gjc8IwZEbyzwYHH1dYfVkVC14GdS40DRhsH4zQIAPiBnrb7Mryj-rTP8vzajdIKH9BpFur6g&gt;  _x000D_
- &lt;http://res.cloudinary.com/degreed/image/fetch/c_lfill,d_broken-image_iufgnh.png,h_150,w_150/https://prod.degreedcdn.com/content/img/org/421/8fdd4f49-016c-4a50-a1f3-9c3f746283b0.jpg%3Fv%3D0010127815&gt; Business perspectives unleashing R&amp;D's potential with William Roze CEO of Capgemini Engineering.… _x000D_
-_x000D_
-Video • 58 Minutes _x000D_
-Learning from Success and Failure &lt;https://email.notifications.degreed.com/c/eJx9kctqwzAQRb_G3hQHPfyIF1oUQlZdFFro0oylsaPGkoweLe7XVwlpSTcFLaQ7XM2dM2g_tHfWoI3i2TuVZNTOliho2_Y9paRjJRrQyxC3FcUb4nnZHl6SMeC3gj8-3Jm0YIQxyki2kbrudzVKmCRvJIzdSDgWNbEu6klLuBjCTuHsEdVOOlOeBGvZnkMzUUaJ3I-AtSKyG5t-ZA3fN02ZAvph9W7SCw5n3AStO0Lbri8XcYpxDTlQwY753H2cX-CjlguGfF0QvNV2ribvTBWSlBhCBVZVUx4yeSz4URX8QFnTNZzwgrXOzyG4rElYZzTa6iymaAaDSieTC1dAN1GCWUHPNssXGhVlFaG3WnDJy9zh8HnF-ONwNmb8WX51CrbwdItY5sZg9deV1aCVqBktvZiTXhb0xu1G8PAOIVP9TXYl-WeT8f-dKbEfObTfgVmvAA&gt;  _x000D_
- &lt;http://res.cloudinary.com/degreed/image/fetch/c_lfill,d_broken-image_iufgnh.png,h_150,w_150/https://hbr.org/resources/images/products/CL-generic-image-hbrarticle.png&gt; One of the mottoes that Diego Rodriguez and I use at the Stanford d.school is "failure sucks, but instructs." We encourage students to learn from the constant stream of small setbacks and successes th… _x000D_
-_x000D_
-Article • 4 Minutes _x000D_
-Did You Know? _x000D_
-Powered by 	 &lt;https://email.notifications.degreed.com/c/eJx9kLtuwzAMRb_GWgIYetmOBg1dOhfo0NGgJMpRo4chywXcr6-bKV0KcLnDIc8l5q9QS06Ym36rxe22hZIJajaOSjFGJ04wQYhzO1bUH4j3eFze95SgHp14uTxBQXPKOeP0xKiUqpdowVsxWDCToQI7SXNpwQcLv8DWO1wqouttSeSmhfAcPR-4uAo7mOskDB294qCodYNAsm9Y57UWHyLOdzw0kxNl46RI1LfW1u0U6vjrOU-Lz0RKXSCH78fVOTgtOSNVL3uIEWsqvYEKn7CdfhbWBVPI4eH05yft__ZOX42A8Qe6dXDq&gt; 	_x000D_
-© 2020-2022 Degreed, All rights reserved_x000D_
-4305 Hacienda Drive, Suite 300, Pleasanton, CA 94588 	_x000D_
-Unsubscribe &lt;https://email.notifications.degreed.com/c/eJx9kE9rhDAQxT-NXpaV_NOYQw6FsudCDz3KmIyaXZNIogX76esutGwvhYFhHvwe8x6GT5di8BhW_Zai3czqYihR06ZRilIiWYke3Nyt-4L6A_E276f3zXtIe8FfTk-Q04wwRhk5MCKEqgQaGAyvDfSyJxwLQUJc3eAM3IFcWRwToq1M9OWk64ZL2hIJjLaKiFogGahRSgwGpYKm3DKmbklxcDN2N9w1FZLQRqpy1tO6Lvl4qGCXY56Mj-vO3VfIW59Ncj0W_DJBngr--mNx5vIsrCVGWKAMaxRKgKTYG0ZFbduB1m3BmpjGnOPBGVhG9C648pAguK9HpM5ZLRgtkx43N8-YfKx6SHCFfIT_ZR6B_xS-_l-t1W3PofkGYpeNCw&gt;  | Update settings &lt;https://email.notifications.degreed.com/c/eJx9UE1rxCAU_DXxshD8SMx68FAoey700GN40Zes3ahBTSH99bULLdtL4fFgYGaYGQwfLsXgMRT9kqLdTXExENRMSqUYowMn6MGtYzk21G-It_U4ve7eQzoa8XR6EDnNKeeM0yqjXafaDg3MRvQGpmGiApuOhljc7Ax8C3JrcUmItjXRk6tm6ixw6i3tzwMHJelsxYyMSzX3EzBJ9oxp3FKc3YrjDQ_NuoEyOSiy6mspW66BGn6p92Bckcf6MpbiwlI5l5iWnGMjng1sC3oXXMNFpVS238NPOlJpENznHY3O6o4zkvSyu3XF5GM7QYJ3yLXVr8-9yZ8ly_-bWX2eBMgvm1CEZQ&gt;  	_x000D_
- &lt;https://email.notifications.degreed.com/o/eJx9j7tuxCAQRb9maVayeAWbgiJ_EClFSmuAwZmsAQvbK3m_Ps5WSZP-Hp1za5ug0AM2qmWk6LQUDJ0wxloheC8ZZqB53I4F3QfibT6u73vO0I6Ler2-tRr38MMycpJLKSQ_Ma617TQGSEG9BPC95wovmpe6UaLwlK1dxKkhxi7UzD7dORbKBBOVxMEYHwcperCG85R8kpbtK7ZxaTXRjOMNDyd0z4XpLcNyp1ZLxrK5X0XNTTvNM7ZcOw8NvmA9GwIsE2Yq9PT-Abb_H0Y3eAXmG7ElZ54&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This mail has been sent from an external source	_x000D_
- &lt;https://prod.degreedcdn.com/content/img/org/421-2c6e3e82-a1cb-4592-bda5-40303fd22fab.png&gt; 	_x000D_
-Hi GUILLERMO, here's your weekly digest	 _x000D_
- &lt;https://prod.degreedcdn.com/content/img/email/babycenter/divider-gray.png&gt; _x000D_
-	_x000D_
-What to Learn Next: _x000D_
-Here's what people at Capgemini NEXT are learning this week 	View All &lt;https://email.notifications.degreed.com/c/eJx9UctqwzAQ_Br7UmL0ihwddAiUnAuF9mgUae2o0cNIcoP79VVCWtJLQYfVDLM7Owvh06YYPIQiX1I0iy42hhYk5lwIjDGnLXhl3VDWGeQ7wNmtT6-L9yqtDd0_PYisJIgQTBDGjAmGOiCgGd4x4Jhve4YahkIsdrRaXQW5MzAlANPp6NuT1L1GggjCtoRSwUYQWitMFdopbWDk7ZIhDXOKo3UwnGGVmPUI8160Tp5KmXM11JBDfQ-N68_DFVL5dIwqmYYeYppyjg191mqewNtgG8KX4gcPxi6-Ered76BWflZ2ChW-LrjBZIPwnctxSRoqc7kl86OIodREK_xm4bJ37lDNNIRWG2Ot2jpfBft1S2GwRjKC2ySnxToHycfuqJL6ULnm9WvwltGfG5X_r2Hk7kgV_wbFL6D7&gt;  	_x000D_
-3 Trends Transforming eLearning Course Design &lt;https://email.notifications.degreed.com/c/eJx9UcFqxCAQ_ZrkUhLUuG5y8FBY9tRDoYUew6xOsnajBjUt6dfXDduyvRQEZ97wZh7vofswwTuLLsnn4PWikvGuREmF6DpKqWhKtGCmPq0zyjfEy7Q-vCzWQliL5vHhjmQkI4xRRijlvOOkRoaK05ajoGK356TgxPlkBqPgSoi1xjEg6lp5W56lBkp2TKESrWjY0A6MaIIAO7brQKuhXCKGfg5-MBP2F1wl5XtCxb4rJ3lOaY5ZUMGO-d0tzh2EZNSEMZdNlQI6HfMHLg4-WOPGCieE4K6V8kuIWGmMZnRFc9RFc2At7_ZZQ8GED2OMPmMK5hEz12RwSba3qM1i82Az6wYqsDNsew5XZyrKKkJvs5gPKcyTz83SH4Z3KUeR4VevYY1PN11lPgzOfG2-9UZLzmgZ5LiYacJgfX2CAO8Qs8O_yjZX_6Sa_s9Py_bUgPgGAVuzpQ&gt;  _x000D_
- &lt;http://res.cloudinary.com/degreed/image/fetch/c_lfill,d_broken-image_iufgnh.png,h_150,w_150/https://gcp-cdn.anderspink.com/article-images/430e5832f89484723fc8bab08afb3270190a990df934a5cf5e00a13e09c5d6dc.jpg&gt; elearningindustry.com | 12 Dec 2021 | Modern digital education is moving toward a more collaborative and inclusive approach. A perfect example is how companies are offering engaging multilingual eLear… _x000D_
-_x000D_
-Article • 4 Minutes _x000D_
-Business perspective - R&amp;D's potential &lt;https://email.notifications.degreed.com/c/eJx9kc1qwzAQhJ_GvhQb6ydydNChUHLqodBCj0a2Ns42lmQkOcV9-iomLemloIM0w2iHb8FdMHhnwSX1ErxZhoTelaCIEFISQgQrwWqcurTOoN4BztP68LpYq8NasMeHuxAq2lBKaEMI55I3NVAYONlzEETsWt4UvHE-4REHfQ3E2sAYAEw9eFueFFAO2uyZ4VKI_kgpbY961wP0kjV7JsslQujm4I84QXeGVRHeNkS0spzUKaU55kIFPeRz93F-XdCAj_nSLxEdxFjNEOIMufYFqlCZKis-ZQaop4IdTMGeGBWESSoLKnwYY_RZG_Q8gkWHWVyS7SwYXGw2NkI3cdB21ji6LF9xVIRWDbl50S9hgOx8bhx_Et5dZ2f5zRu9xmfQwaEbyzxYO_zaYHVoFKekDGpccJogWF_3OugPHTPW32Ybyj-rTP8vzah9z7T4Bo9drxY&gt;  _x000D_
- &lt;http://res.cloudinary.com/degreed/image/fetch/c_lfill,d_broken-image_iufgnh.png,h_150,w_150/https://prod.degreedcdn.com/content/img/org/421/8fdd4f49-016c-4a50-a1f3-9c3f746283b0.jpg%3Fv%3D0010127815&gt; Business perspectives unleashing R&amp;D's potential with William Roze CEO of Capgemini Engineering.… _x000D_
-_x000D_
-Video • 58 Minutes _x000D_
-Learning from Success and Failure &lt;https://email.notifications.degreed.com/c/eJx9kT9vwyAQxT-NvVS2OIztZGCoFGXqUKmVOloEzg6NAYs_rdxPX2KlVbpUYoB3ety736H90N5ZgzbyZ-9UklE7WyKHrtvvAaBrSjRCz0NcF-RviJd5fXhJxgi_Fs3jw51Jc0ooBUoAGNszUiNFyWDHsIOu7RkpGLEu6lFLcTWEWuHkEVUtnSnPvB2btu9bQHLqBVWjakckVJEdI0T1OyhTQD8s3o16xuGCKwfWE-j6fTnzc4xLyIEKeszn7uP8Ej5qOWPI1xmFt9pO1eidqUKSEkOohFXVmIdMHovmqIrmALTt24Y0Be2cn0JwWZNimdBoq7OYohkMKp1MLmyAbqIUZhF6slm-0qiAVgRuteCSl7nD4XPD-ONwNmb8WX51Sqzh6RaxzI2F1V8bq0ErziiUnk9JzzN64-qT8OJdhEz1N9lG8s8m4_87U3x3akT3DRaAriY&gt;  _x000D_
- &lt;http://res.cloudinary.com/degreed/image/fetch/c_lfill,d_broken-image_iufgnh.png,h_150,w_150/https://hbr.org/resources/images/products/CL-generic-image-hbrarticle.png&gt; One of the mottoes that Diego Rodriguez and I use at the Stanford d.school is "failure sucks, but instructs." We encourage students to learn from the constant stream of small setbacks and successes th… _x000D_
-_x000D_
-Article • 4 Minutes _x000D_
-Did You Know? _x000D_
-Powered by 	 &lt;https://email.notifications.degreed.com/c/eJx9kLtuxCAQRb_GNCtZDGYxFBRpUkdKkdLCMHjJ8rAwjuR8fZytNk2kaaY4954ZzF-hlpwwN_1Wi9ttCyUT1CCEUgAgBoLJhDi1Y0X9gXiPx-V9T8nUoxteLk9Q0IwyBowCcK447ZGh5SA5ChDXkdOO01xa8MGaX2DrHS4V0fW2JHLTg1Ae0Htnpb1KP6JzarbC4SCtdxLIvmGd1lp8iDjd8dDARwpiVCTqW2vrdgp17PWcp-BzI6UuJofvR-sUnOYMSNXLHmLEmko_m2o-zXb6WbMumEIOD6c_P2n_X--0nAcjfgDI9HFK&gt; 	_x000D_
-© 2020-2022 Degreed, All rights reserved_x000D_
-4305 Hacienda Drive, Suite 300, Pleasanton, CA 94588 	_x000D_
-Unsubscribe &lt;https://email.notifications.degreed.com/c/eJx9kMFqhDAQhp9GL2UlM8aohxwKZc-FHnqUMRnddDWRRAv26esutGwvhYFhBr6f-Yb9p4vBz-xX_RqD3czqgs9Zg1JtCwCqzHkmN3XrvrB-Z75O-9PbNs8U96x8fnqAnEaBCCgApGylKBjZSGgkK1BVLUUmhQ-rG5yhG5AKy2NktoUJc37RdhCl6rGqaEBqGaiWYNtemQZFjdjmW-LYLTEMbuLuyrsGWQtQdZtP-rKuSzoOyvB81EPwMd24W_Np65OJruesPF8oXbLy5SfiVNYnaa0w0hIgV3wYUA3cGwRZ2WaAqslQhTimFA7O0DLy7LzLjxV593VX6pzVEiGPetzcNHGcQ9FTpA9Kh_wvcxf-8_D1_9da3fQlqW-e14x5&gt;  | Update settings &lt;https://email.notifications.degreed.com/c/eJx9UMtqwzAQ_BrrEjCrR-X4oEOh5FzooUezljeOEksyklxwv75qoCW9FJaFgZlhZih8uBSDp1DMa4rTZouLgZHhWvc951xLRh7dMpR9JfNOdFv2w9vmPaa9kc-HB5EzAoTgAjhXqlfQkiCr-FGR5vqpU9AoCLG4s7P4LcjtRHMimlobPbsYSQAwAqiOg8UOrewknMlaQNKIR7ZlSsOa4tktNNxoN1x1wHXXs8VcSllzDdSIU70H44o81ZepFBfmyjnFNOccG_licZ3Ju-AaISulsv0WftKxSsPgPu9ocJNRgrNk5s0tCyUf2xETXjHXVr8-9yZ_liz_bzaZ4yhRfwG8M4O2&gt;  	_x000D_
- &lt;https://email.notifications.degreed.com/o/eJx9jzFuxCAQAF9zNCdZLOxhU1DkB5FSpLQwLM7mDFjYjuS8PslVSZMHjGamttkX_vQ71zJydKhAkANjrAUAowVlz8u4nyu5V6L7cl5fjpx9Oy_66frcajzCDyvYKakUKAmAaFF2pCggDEgGzK1HeUFZ6s6Jw0O2dZHmRhS7ULN4cyl4sFprUjEN3hLeKEJKkRSmYUIjjo3auLaaeKHxTqcD7CWY3goqH9xqyVR296uoufngZaGWazf55t_99t0Q_DpT5sIP7x9g__8wumHS3nwBMSJnJw&gt; </t>
   </si>
 </sst>
 </file>
@@ -547,83 +457,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2">
-        <v>44896.435243055559</v>
-      </c>
-      <c r="H2" s="2">
-        <v>44896.435243055559</v>
-      </c>
-      <c r="I2" s="2">
-        <v>44896.435243055559</v>
-      </c>
-      <c r="J2" s="2">
-        <v>44896.435243055559</v>
-      </c>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F2" s="1"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2">
-        <v>44896.425405092596</v>
-      </c>
-      <c r="H3" s="2">
-        <v>44896.425405092596</v>
-      </c>
-      <c r="I3" s="2">
-        <v>44896.425405092596</v>
-      </c>
-      <c r="J3" s="2">
-        <v>44896.425405092596</v>
-      </c>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="2">
-        <v>44896.425567129627</v>
-      </c>
-      <c r="H4" s="2">
-        <v>44896.425567129627</v>
-      </c>
-      <c r="I4" s="2">
-        <v>44896.425567129627</v>
-      </c>
-      <c r="J4" s="2">
-        <v>44896.425567129627</v>
-      </c>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F4" s="1"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>